<commit_message>
Added trilogy based calculations of 2018 chlorophyll-a. Fixed two entry based erorrs for PAR and DO. Moves some files around to clean up project structure.
</commit_message>
<xml_diff>
--- a/2019 chla/Chla_C7_curve.xlsx
+++ b/2019 chla/Chla_C7_curve.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kellyloria/Documents/Niwot LTER 2017-2019/GeneralQ/General_QAQC/2019 chla/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2504CF9E-5706-8441-950A-3AAAD3A0C9BB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E93C4A22-57DB-504B-BB7A-C1135E86223B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5260" yWindow="1840" windowWidth="27640" windowHeight="15960" xr2:uid="{5C5212B1-2F60-544B-B060-D768D0F8CD42}"/>
+    <workbookView xWindow="8960" yWindow="4160" windowWidth="27640" windowHeight="15960" xr2:uid="{5C5212B1-2F60-544B-B060-D768D0F8CD42}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029" refMode="R1C1"/>
+  <calcPr calcId="191029" refMode="R1C1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,7 +23,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>

</xml_diff>